<commit_message>
Change dato to unique plant_id
</commit_message>
<xml_diff>
--- a/test/cases/small_data.xlsx
+++ b/test/cases/small_data.xlsx
@@ -184,12 +184,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -217,2847 +221,2847 @@
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
         <v>184</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>44875</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="L2" s="0" t="n">
+      <c r="C2" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="L2" s="2" t="n">
         <v>100358904</v>
       </c>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2" t="n">
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3" t="n">
         <v>44875.0034998148</v>
       </c>
-      <c r="AC2" s="0" t="n">
+      <c r="AC2" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
         <v>183</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>44875</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="I3" s="0" t="n">
+      <c r="C3" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="2" t="n">
         <v>14.1</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="2" t="n">
         <v>112809400</v>
       </c>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2" t="n">
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3" t="n">
         <v>44875.0034996991</v>
       </c>
-      <c r="AC3" s="0" t="n">
+      <c r="AC3" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
         <v>184</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>44875.0034722222</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="I4" s="0" t="n">
+      <c r="C4" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="2" t="n">
         <v>15.1</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="2" t="n">
         <v>100358904</v>
       </c>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2" t="n">
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3" t="n">
         <v>44875.0069787037</v>
       </c>
-      <c r="AC4" s="0" t="n">
+      <c r="AC4" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
         <v>183</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>44875.0034722222</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="L5" s="0" t="n">
+      <c r="C5" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="L5" s="2" t="n">
         <v>112809400</v>
       </c>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2" t="n">
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3" t="n">
         <v>44875.0069785764</v>
       </c>
-      <c r="AC5" s="0" t="n">
+      <c r="AC5" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
         <v>184</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>44875.0069444445</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="I6" s="0" t="n">
+      <c r="C6" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="2" t="n">
         <v>15.1</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6" s="2" t="n">
         <v>100358904</v>
       </c>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2" t="n">
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3" t="n">
         <v>44875.010446331</v>
       </c>
-      <c r="AC6" s="0" t="n">
+      <c r="AC6" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
         <v>183</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>44875.0069444445</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="I7" s="0" t="n">
+      <c r="C7" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="2" t="n">
         <v>14.1</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="2" t="n">
         <v>112809400</v>
       </c>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2" t="n">
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3" t="n">
         <v>44875.0104462153</v>
       </c>
-      <c r="AC7" s="0" t="n">
+      <c r="AC7" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
         <v>184</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>44875.0104166667</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="I8" s="0" t="n">
+      <c r="C8" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="2" t="n">
         <v>15.1</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8" s="2" t="n">
         <v>100358904</v>
       </c>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2" t="n">
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3" t="n">
         <v>44875.0139142245</v>
       </c>
-      <c r="AC8" s="0" t="n">
+      <c r="AC8" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
         <v>183</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>44875.0104166667</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="I9" s="0" t="n">
+      <c r="C9" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="2" t="n">
         <v>14.1</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9" s="2" t="n">
         <v>112809400</v>
       </c>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2" t="n">
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3" t="n">
         <v>44875.0139140625</v>
       </c>
-      <c r="AC9" s="0" t="n">
+      <c r="AC9" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
         <v>184</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>44875.0138888889</v>
       </c>
-      <c r="C10" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="I10" s="0" t="n">
+      <c r="C10" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="2" t="n">
         <v>15.1</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10" s="2" t="n">
         <v>100358904</v>
       </c>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2" t="n">
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3" t="n">
         <v>44875.0173932176</v>
       </c>
-      <c r="AC10" s="0" t="n">
+      <c r="AC10" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
         <v>183</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>44875.0138888889</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>31</v>
-      </c>
-      <c r="L11" s="0" t="n">
+      <c r="C11" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="L11" s="2" t="n">
         <v>112809400</v>
       </c>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="2" t="n">
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3" t="n">
         <v>44875.0173930787</v>
       </c>
-      <c r="AC11" s="0" t="n">
+      <c r="AC11" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z12" s="2"/>
+      <c r="Z12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z13" s="2"/>
+      <c r="Z13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z14" s="2"/>
+      <c r="Z14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z15" s="2"/>
+      <c r="Z15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z16" s="2"/>
+      <c r="Z16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z17" s="2"/>
+      <c r="Z17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z18" s="2"/>
+      <c r="Z18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z19" s="2"/>
+      <c r="Z19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z20" s="2"/>
+      <c r="Z20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z21" s="2"/>
+      <c r="Z21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z22" s="2"/>
+      <c r="Z22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z23" s="2"/>
+      <c r="Z23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z24" s="2"/>
+      <c r="Z24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z25" s="2"/>
+      <c r="Z25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z26" s="2"/>
+      <c r="Z26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z27" s="2"/>
+      <c r="Z27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z28" s="2"/>
+      <c r="Z28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z29" s="2"/>
+      <c r="Z29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z30" s="2"/>
+      <c r="Z30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z31" s="2"/>
+      <c r="Z31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z32" s="2"/>
+      <c r="Z32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z33" s="2"/>
+      <c r="Z33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z34" s="2"/>
+      <c r="Z34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z35" s="2"/>
+      <c r="Z35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z36" s="2"/>
+      <c r="Z36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z37" s="2"/>
+      <c r="Z37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z38" s="2"/>
+      <c r="Z38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z39" s="2"/>
+      <c r="Z39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z40" s="2"/>
+      <c r="Z40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z41" s="2"/>
+      <c r="Z41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z42" s="2"/>
+      <c r="Z42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z43" s="2"/>
+      <c r="Z43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z44" s="2"/>
+      <c r="Z44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z45" s="2"/>
+      <c r="Z45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z46" s="2"/>
+      <c r="Z46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z47" s="2"/>
+      <c r="Z47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z48" s="2"/>
+      <c r="Z48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z49" s="2"/>
+      <c r="Z49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z50" s="2"/>
+      <c r="Z50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z51" s="2"/>
+      <c r="Z51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z52" s="2"/>
+      <c r="Z52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z53" s="2"/>
+      <c r="Z53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z54" s="2"/>
+      <c r="Z54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z55" s="2"/>
+      <c r="Z55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z56" s="2"/>
+      <c r="Z56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z57" s="2"/>
+      <c r="Z57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z58" s="2"/>
+      <c r="Z58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z59" s="2"/>
+      <c r="Z59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z60" s="2"/>
+      <c r="Z60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z61" s="2"/>
+      <c r="Z61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z62" s="2"/>
+      <c r="Z62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z63" s="2"/>
+      <c r="Z63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z64" s="2"/>
+      <c r="Z64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z65" s="2"/>
+      <c r="Z65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z66" s="2"/>
+      <c r="Z66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z67" s="2"/>
+      <c r="Z67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z68" s="2"/>
+      <c r="Z68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z69" s="2"/>
+      <c r="Z69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z70" s="2"/>
+      <c r="Z70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z71" s="2"/>
+      <c r="Z71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z72" s="2"/>
+      <c r="Z72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z73" s="2"/>
+      <c r="Z73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z74" s="2"/>
+      <c r="Z74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z75" s="2"/>
+      <c r="Z75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z76" s="2"/>
+      <c r="Z76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z77" s="2"/>
+      <c r="Z77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z78" s="2"/>
+      <c r="Z78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z79" s="2"/>
+      <c r="Z79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z80" s="2"/>
+      <c r="Z80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z81" s="2"/>
+      <c r="Z81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z82" s="2"/>
+      <c r="Z82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z83" s="2"/>
+      <c r="Z83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z84" s="2"/>
+      <c r="Z84" s="3"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z85" s="2"/>
+      <c r="Z85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z86" s="2"/>
+      <c r="Z86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z87" s="2"/>
+      <c r="Z87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z88" s="2"/>
+      <c r="Z88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z89" s="2"/>
+      <c r="Z89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z90" s="2"/>
+      <c r="Z90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z91" s="2"/>
+      <c r="Z91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z92" s="2"/>
+      <c r="Z92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z93" s="2"/>
+      <c r="Z93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z94" s="2"/>
+      <c r="Z94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z95" s="2"/>
+      <c r="Z95" s="3"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z96" s="2"/>
+      <c r="Z96" s="3"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z97" s="2"/>
+      <c r="Z97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z98" s="2"/>
+      <c r="Z98" s="3"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z99" s="2"/>
+      <c r="Z99" s="3"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z100" s="2"/>
+      <c r="Z100" s="3"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z101" s="2"/>
+      <c r="Z101" s="3"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z102" s="2"/>
+      <c r="Z102" s="3"/>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z103" s="2"/>
+      <c r="Z103" s="3"/>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z104" s="2"/>
+      <c r="Z104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z105" s="2"/>
+      <c r="Z105" s="3"/>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z106" s="2"/>
+      <c r="Z106" s="3"/>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z107" s="2"/>
+      <c r="Z107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z108" s="2"/>
+      <c r="Z108" s="3"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z109" s="2"/>
+      <c r="Z109" s="3"/>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z110" s="2"/>
+      <c r="Z110" s="3"/>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z111" s="2"/>
+      <c r="Z111" s="3"/>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z112" s="2"/>
+      <c r="Z112" s="3"/>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z113" s="2"/>
+      <c r="Z113" s="3"/>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z114" s="2"/>
+      <c r="Z114" s="3"/>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z115" s="2"/>
+      <c r="Z115" s="3"/>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z116" s="2"/>
+      <c r="Z116" s="3"/>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z117" s="2"/>
+      <c r="Z117" s="3"/>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z118" s="2"/>
+      <c r="Z118" s="3"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z119" s="2"/>
+      <c r="Z119" s="3"/>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z120" s="2"/>
+      <c r="Z120" s="3"/>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z121" s="2"/>
+      <c r="Z121" s="3"/>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z122" s="2"/>
+      <c r="Z122" s="3"/>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z123" s="2"/>
+      <c r="Z123" s="3"/>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z124" s="2"/>
+      <c r="Z124" s="3"/>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z125" s="2"/>
+      <c r="Z125" s="3"/>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z126" s="2"/>
+      <c r="Z126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z127" s="2"/>
+      <c r="Z127" s="3"/>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z128" s="2"/>
+      <c r="Z128" s="3"/>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z129" s="2"/>
+      <c r="Z129" s="3"/>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z130" s="2"/>
+      <c r="Z130" s="3"/>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z131" s="2"/>
+      <c r="Z131" s="3"/>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z132" s="2"/>
+      <c r="Z132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z133" s="2"/>
+      <c r="Z133" s="3"/>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z134" s="2"/>
+      <c r="Z134" s="3"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z135" s="2"/>
+      <c r="Z135" s="3"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z136" s="2"/>
+      <c r="Z136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z137" s="2"/>
+      <c r="Z137" s="3"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z138" s="2"/>
+      <c r="Z138" s="3"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z139" s="2"/>
+      <c r="Z139" s="3"/>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z140" s="2"/>
+      <c r="Z140" s="3"/>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z141" s="2"/>
+      <c r="Z141" s="3"/>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z142" s="2"/>
+      <c r="Z142" s="3"/>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z143" s="2"/>
+      <c r="Z143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z144" s="2"/>
+      <c r="Z144" s="3"/>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z145" s="2"/>
+      <c r="Z145" s="3"/>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z146" s="2"/>
+      <c r="Z146" s="3"/>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z147" s="2"/>
+      <c r="Z147" s="3"/>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z148" s="2"/>
+      <c r="Z148" s="3"/>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z149" s="2"/>
+      <c r="Z149" s="3"/>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z150" s="2"/>
+      <c r="Z150" s="3"/>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z151" s="2"/>
+      <c r="Z151" s="3"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z152" s="2"/>
+      <c r="Z152" s="3"/>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z153" s="2"/>
+      <c r="Z153" s="3"/>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z154" s="2"/>
+      <c r="Z154" s="3"/>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z155" s="2"/>
+      <c r="Z155" s="3"/>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z156" s="2"/>
+      <c r="Z156" s="3"/>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z157" s="2"/>
+      <c r="Z157" s="3"/>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z158" s="2"/>
+      <c r="Z158" s="3"/>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z159" s="2"/>
+      <c r="Z159" s="3"/>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z160" s="2"/>
+      <c r="Z160" s="3"/>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z161" s="2"/>
+      <c r="Z161" s="3"/>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z162" s="2"/>
+      <c r="Z162" s="3"/>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z163" s="2"/>
+      <c r="Z163" s="3"/>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z164" s="2"/>
+      <c r="Z164" s="3"/>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z165" s="2"/>
+      <c r="Z165" s="3"/>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z166" s="2"/>
+      <c r="Z166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z167" s="2"/>
+      <c r="Z167" s="3"/>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z168" s="2"/>
+      <c r="Z168" s="3"/>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z169" s="2"/>
+      <c r="Z169" s="3"/>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z170" s="2"/>
+      <c r="Z170" s="3"/>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z171" s="2"/>
+      <c r="Z171" s="3"/>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z172" s="2"/>
+      <c r="Z172" s="3"/>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z173" s="2"/>
+      <c r="Z173" s="3"/>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z174" s="2"/>
+      <c r="Z174" s="3"/>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z175" s="2"/>
+      <c r="Z175" s="3"/>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z176" s="2"/>
+      <c r="Z176" s="3"/>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z177" s="2"/>
+      <c r="Z177" s="3"/>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z178" s="2"/>
+      <c r="Z178" s="3"/>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z179" s="2"/>
+      <c r="Z179" s="3"/>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z180" s="2"/>
+      <c r="Z180" s="3"/>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z181" s="2"/>
+      <c r="Z181" s="3"/>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z182" s="2"/>
+      <c r="Z182" s="3"/>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z183" s="2"/>
+      <c r="Z183" s="3"/>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z184" s="2"/>
+      <c r="Z184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z185" s="2"/>
+      <c r="Z185" s="3"/>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z186" s="2"/>
+      <c r="Z186" s="3"/>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z187" s="2"/>
+      <c r="Z187" s="3"/>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z188" s="2"/>
+      <c r="Z188" s="3"/>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z189" s="2"/>
+      <c r="Z189" s="3"/>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z190" s="2"/>
+      <c r="Z190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z191" s="2"/>
+      <c r="Z191" s="3"/>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z192" s="2"/>
+      <c r="Z192" s="3"/>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z193" s="2"/>
+      <c r="Z193" s="3"/>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z194" s="2"/>
+      <c r="Z194" s="3"/>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z195" s="2"/>
+      <c r="Z195" s="3"/>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z196" s="2"/>
+      <c r="Z196" s="3"/>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z197" s="2"/>
+      <c r="Z197" s="3"/>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z198" s="2"/>
+      <c r="Z198" s="3"/>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z199" s="2"/>
+      <c r="Z199" s="3"/>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z200" s="2"/>
+      <c r="Z200" s="3"/>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z201" s="2"/>
+      <c r="Z201" s="3"/>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z202" s="2"/>
+      <c r="Z202" s="3"/>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z203" s="2"/>
+      <c r="Z203" s="3"/>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z204" s="2"/>
+      <c r="Z204" s="3"/>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z205" s="2"/>
+      <c r="Z205" s="3"/>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z206" s="2"/>
+      <c r="Z206" s="3"/>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z207" s="2"/>
+      <c r="Z207" s="3"/>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z208" s="2"/>
+      <c r="Z208" s="3"/>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z209" s="2"/>
+      <c r="Z209" s="3"/>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z210" s="2"/>
+      <c r="Z210" s="3"/>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z211" s="2"/>
+      <c r="Z211" s="3"/>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z212" s="2"/>
+      <c r="Z212" s="3"/>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z213" s="2"/>
+      <c r="Z213" s="3"/>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z214" s="2"/>
+      <c r="Z214" s="3"/>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z215" s="2"/>
+      <c r="Z215" s="3"/>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z216" s="2"/>
+      <c r="Z216" s="3"/>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z217" s="2"/>
+      <c r="Z217" s="3"/>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z218" s="2"/>
+      <c r="Z218" s="3"/>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z219" s="2"/>
+      <c r="Z219" s="3"/>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z220" s="2"/>
+      <c r="Z220" s="3"/>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z221" s="2"/>
+      <c r="Z221" s="3"/>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z222" s="2"/>
+      <c r="Z222" s="3"/>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z223" s="2"/>
+      <c r="Z223" s="3"/>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z224" s="2"/>
+      <c r="Z224" s="3"/>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z225" s="2"/>
+      <c r="Z225" s="3"/>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z226" s="2"/>
+      <c r="Z226" s="3"/>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z227" s="2"/>
+      <c r="Z227" s="3"/>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z228" s="2"/>
+      <c r="Z228" s="3"/>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z229" s="2"/>
+      <c r="Z229" s="3"/>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z230" s="2"/>
+      <c r="Z230" s="3"/>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z231" s="2"/>
+      <c r="Z231" s="3"/>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z232" s="2"/>
+      <c r="Z232" s="3"/>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z233" s="2"/>
+      <c r="Z233" s="3"/>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z234" s="2"/>
+      <c r="Z234" s="3"/>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z235" s="2"/>
+      <c r="Z235" s="3"/>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z236" s="2"/>
+      <c r="Z236" s="3"/>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z237" s="2"/>
+      <c r="Z237" s="3"/>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z238" s="2"/>
+      <c r="Z238" s="3"/>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z239" s="2"/>
+      <c r="Z239" s="3"/>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z240" s="2"/>
+      <c r="Z240" s="3"/>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z241" s="2"/>
+      <c r="Z241" s="3"/>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z242" s="2"/>
+      <c r="Z242" s="3"/>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z243" s="2"/>
+      <c r="Z243" s="3"/>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z244" s="2"/>
+      <c r="Z244" s="3"/>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z245" s="2"/>
+      <c r="Z245" s="3"/>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z246" s="2"/>
+      <c r="Z246" s="3"/>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z247" s="2"/>
+      <c r="Z247" s="3"/>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z248" s="2"/>
+      <c r="Z248" s="3"/>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z249" s="2"/>
+      <c r="Z249" s="3"/>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z250" s="2"/>
+      <c r="Z250" s="3"/>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z251" s="2"/>
+      <c r="Z251" s="3"/>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z252" s="2"/>
+      <c r="Z252" s="3"/>
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z253" s="2"/>
+      <c r="Z253" s="3"/>
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z254" s="2"/>
+      <c r="Z254" s="3"/>
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z255" s="2"/>
+      <c r="Z255" s="3"/>
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z256" s="2"/>
+      <c r="Z256" s="3"/>
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z257" s="2"/>
+      <c r="Z257" s="3"/>
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z258" s="2"/>
+      <c r="Z258" s="3"/>
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z259" s="2"/>
+      <c r="Z259" s="3"/>
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z260" s="2"/>
+      <c r="Z260" s="3"/>
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z261" s="2"/>
+      <c r="Z261" s="3"/>
     </row>
     <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z262" s="2"/>
+      <c r="Z262" s="3"/>
     </row>
     <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z263" s="2"/>
+      <c r="Z263" s="3"/>
     </row>
     <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z264" s="2"/>
+      <c r="Z264" s="3"/>
     </row>
     <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z265" s="2"/>
+      <c r="Z265" s="3"/>
     </row>
     <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z266" s="2"/>
+      <c r="Z266" s="3"/>
     </row>
     <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z267" s="2"/>
+      <c r="Z267" s="3"/>
     </row>
     <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z268" s="2"/>
+      <c r="Z268" s="3"/>
     </row>
     <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z269" s="2"/>
+      <c r="Z269" s="3"/>
     </row>
     <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z270" s="2"/>
+      <c r="Z270" s="3"/>
     </row>
     <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z271" s="2"/>
+      <c r="Z271" s="3"/>
     </row>
     <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z272" s="2"/>
+      <c r="Z272" s="3"/>
     </row>
     <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z273" s="2"/>
+      <c r="Z273" s="3"/>
     </row>
     <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z274" s="2"/>
+      <c r="Z274" s="3"/>
     </row>
     <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z275" s="2"/>
+      <c r="Z275" s="3"/>
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z276" s="2"/>
+      <c r="Z276" s="3"/>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z277" s="2"/>
+      <c r="Z277" s="3"/>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z278" s="2"/>
+      <c r="Z278" s="3"/>
     </row>
     <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z279" s="2"/>
+      <c r="Z279" s="3"/>
     </row>
     <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z280" s="2"/>
+      <c r="Z280" s="3"/>
     </row>
     <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z281" s="2"/>
+      <c r="Z281" s="3"/>
     </row>
     <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z282" s="2"/>
+      <c r="Z282" s="3"/>
     </row>
     <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z283" s="2"/>
+      <c r="Z283" s="3"/>
     </row>
     <row r="284" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z284" s="2"/>
+      <c r="Z284" s="3"/>
     </row>
     <row r="285" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z285" s="2"/>
+      <c r="Z285" s="3"/>
     </row>
     <row r="286" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z286" s="2"/>
+      <c r="Z286" s="3"/>
     </row>
     <row r="287" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z287" s="2"/>
+      <c r="Z287" s="3"/>
     </row>
     <row r="288" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z288" s="2"/>
+      <c r="Z288" s="3"/>
     </row>
     <row r="289" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z289" s="2"/>
+      <c r="Z289" s="3"/>
     </row>
     <row r="290" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z290" s="2"/>
+      <c r="Z290" s="3"/>
     </row>
     <row r="291" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z291" s="2"/>
+      <c r="Z291" s="3"/>
     </row>
     <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z292" s="2"/>
+      <c r="Z292" s="3"/>
     </row>
     <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z293" s="2"/>
+      <c r="Z293" s="3"/>
     </row>
     <row r="294" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z294" s="2"/>
+      <c r="Z294" s="3"/>
     </row>
     <row r="295" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z295" s="2"/>
+      <c r="Z295" s="3"/>
     </row>
     <row r="296" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z296" s="2"/>
+      <c r="Z296" s="3"/>
     </row>
     <row r="297" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z297" s="2"/>
+      <c r="Z297" s="3"/>
     </row>
     <row r="298" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z298" s="2"/>
+      <c r="Z298" s="3"/>
     </row>
     <row r="299" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z299" s="2"/>
+      <c r="Z299" s="3"/>
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z300" s="2"/>
+      <c r="Z300" s="3"/>
     </row>
     <row r="301" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z301" s="2"/>
+      <c r="Z301" s="3"/>
     </row>
     <row r="302" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z302" s="2"/>
+      <c r="Z302" s="3"/>
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z303" s="2"/>
+      <c r="Z303" s="3"/>
     </row>
     <row r="304" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z304" s="2"/>
+      <c r="Z304" s="3"/>
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z305" s="2"/>
+      <c r="Z305" s="3"/>
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z306" s="2"/>
+      <c r="Z306" s="3"/>
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z307" s="2"/>
+      <c r="Z307" s="3"/>
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z308" s="2"/>
+      <c r="Z308" s="3"/>
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z309" s="2"/>
+      <c r="Z309" s="3"/>
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z310" s="2"/>
+      <c r="Z310" s="3"/>
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z311" s="2"/>
+      <c r="Z311" s="3"/>
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z312" s="2"/>
+      <c r="Z312" s="3"/>
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z313" s="2"/>
+      <c r="Z313" s="3"/>
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z314" s="2"/>
+      <c r="Z314" s="3"/>
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z315" s="2"/>
+      <c r="Z315" s="3"/>
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z316" s="2"/>
+      <c r="Z316" s="3"/>
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z317" s="2"/>
+      <c r="Z317" s="3"/>
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z318" s="2"/>
+      <c r="Z318" s="3"/>
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z319" s="2"/>
+      <c r="Z319" s="3"/>
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z320" s="2"/>
+      <c r="Z320" s="3"/>
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z321" s="2"/>
+      <c r="Z321" s="3"/>
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z322" s="2"/>
+      <c r="Z322" s="3"/>
     </row>
     <row r="323" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z323" s="2"/>
+      <c r="Z323" s="3"/>
     </row>
     <row r="324" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z324" s="2"/>
+      <c r="Z324" s="3"/>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z325" s="2"/>
+      <c r="Z325" s="3"/>
     </row>
     <row r="326" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z326" s="2"/>
+      <c r="Z326" s="3"/>
     </row>
     <row r="327" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z327" s="2"/>
+      <c r="Z327" s="3"/>
     </row>
     <row r="328" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z328" s="2"/>
+      <c r="Z328" s="3"/>
     </row>
     <row r="329" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z329" s="2"/>
+      <c r="Z329" s="3"/>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z330" s="2"/>
+      <c r="Z330" s="3"/>
     </row>
     <row r="331" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z331" s="2"/>
+      <c r="Z331" s="3"/>
     </row>
     <row r="332" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z332" s="2"/>
+      <c r="Z332" s="3"/>
     </row>
     <row r="333" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z333" s="2"/>
+      <c r="Z333" s="3"/>
     </row>
     <row r="334" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z334" s="2"/>
+      <c r="Z334" s="3"/>
     </row>
     <row r="335" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z335" s="2"/>
+      <c r="Z335" s="3"/>
     </row>
     <row r="336" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z336" s="2"/>
+      <c r="Z336" s="3"/>
     </row>
     <row r="337" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z337" s="2"/>
+      <c r="Z337" s="3"/>
     </row>
     <row r="338" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z338" s="2"/>
+      <c r="Z338" s="3"/>
     </row>
     <row r="339" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z339" s="2"/>
+      <c r="Z339" s="3"/>
     </row>
     <row r="340" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z340" s="2"/>
+      <c r="Z340" s="3"/>
     </row>
     <row r="341" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z341" s="2"/>
+      <c r="Z341" s="3"/>
     </row>
     <row r="342" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z342" s="2"/>
+      <c r="Z342" s="3"/>
     </row>
     <row r="343" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z343" s="2"/>
+      <c r="Z343" s="3"/>
     </row>
     <row r="344" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z344" s="2"/>
+      <c r="Z344" s="3"/>
     </row>
     <row r="345" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z345" s="2"/>
+      <c r="Z345" s="3"/>
     </row>
     <row r="346" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z346" s="2"/>
+      <c r="Z346" s="3"/>
     </row>
     <row r="347" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z347" s="2"/>
+      <c r="Z347" s="3"/>
     </row>
     <row r="348" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z348" s="2"/>
+      <c r="Z348" s="3"/>
     </row>
     <row r="349" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z349" s="2"/>
+      <c r="Z349" s="3"/>
     </row>
     <row r="350" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z350" s="2"/>
+      <c r="Z350" s="3"/>
     </row>
     <row r="351" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z351" s="2"/>
+      <c r="Z351" s="3"/>
     </row>
     <row r="352" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z352" s="2"/>
+      <c r="Z352" s="3"/>
     </row>
     <row r="353" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z353" s="2"/>
+      <c r="Z353" s="3"/>
     </row>
     <row r="354" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z354" s="2"/>
+      <c r="Z354" s="3"/>
     </row>
     <row r="355" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z355" s="2"/>
+      <c r="Z355" s="3"/>
     </row>
     <row r="356" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z356" s="2"/>
+      <c r="Z356" s="3"/>
     </row>
     <row r="357" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z357" s="2"/>
+      <c r="Z357" s="3"/>
     </row>
     <row r="358" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z358" s="2"/>
+      <c r="Z358" s="3"/>
     </row>
     <row r="359" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z359" s="2"/>
+      <c r="Z359" s="3"/>
     </row>
     <row r="360" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z360" s="2"/>
+      <c r="Z360" s="3"/>
     </row>
     <row r="361" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z361" s="2"/>
+      <c r="Z361" s="3"/>
     </row>
     <row r="362" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z362" s="2"/>
+      <c r="Z362" s="3"/>
     </row>
     <row r="363" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z363" s="2"/>
+      <c r="Z363" s="3"/>
     </row>
     <row r="364" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z364" s="2"/>
+      <c r="Z364" s="3"/>
     </row>
     <row r="365" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z365" s="2"/>
+      <c r="Z365" s="3"/>
     </row>
     <row r="366" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z366" s="2"/>
+      <c r="Z366" s="3"/>
     </row>
     <row r="367" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z367" s="2"/>
+      <c r="Z367" s="3"/>
     </row>
     <row r="368" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z368" s="2"/>
+      <c r="Z368" s="3"/>
     </row>
     <row r="369" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z369" s="2"/>
+      <c r="Z369" s="3"/>
     </row>
     <row r="370" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z370" s="2"/>
+      <c r="Z370" s="3"/>
     </row>
     <row r="371" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z371" s="2"/>
+      <c r="Z371" s="3"/>
     </row>
     <row r="372" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z372" s="2"/>
+      <c r="Z372" s="3"/>
     </row>
     <row r="373" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z373" s="2"/>
+      <c r="Z373" s="3"/>
     </row>
     <row r="374" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z374" s="2"/>
+      <c r="Z374" s="3"/>
     </row>
     <row r="375" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z375" s="2"/>
+      <c r="Z375" s="3"/>
     </row>
     <row r="376" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z376" s="2"/>
+      <c r="Z376" s="3"/>
     </row>
     <row r="377" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z377" s="2"/>
+      <c r="Z377" s="3"/>
     </row>
     <row r="378" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z378" s="2"/>
+      <c r="Z378" s="3"/>
     </row>
     <row r="379" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z379" s="2"/>
+      <c r="Z379" s="3"/>
     </row>
     <row r="380" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z380" s="2"/>
+      <c r="Z380" s="3"/>
     </row>
     <row r="381" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z381" s="2"/>
+      <c r="Z381" s="3"/>
     </row>
     <row r="382" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z382" s="2"/>
+      <c r="Z382" s="3"/>
     </row>
     <row r="383" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z383" s="2"/>
+      <c r="Z383" s="3"/>
     </row>
     <row r="384" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z384" s="2"/>
+      <c r="Z384" s="3"/>
     </row>
     <row r="385" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z385" s="2"/>
+      <c r="Z385" s="3"/>
     </row>
     <row r="386" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z386" s="2"/>
+      <c r="Z386" s="3"/>
     </row>
     <row r="387" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z387" s="2"/>
+      <c r="Z387" s="3"/>
     </row>
     <row r="388" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z388" s="2"/>
+      <c r="Z388" s="3"/>
     </row>
     <row r="389" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z389" s="2"/>
+      <c r="Z389" s="3"/>
     </row>
     <row r="390" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z390" s="2"/>
+      <c r="Z390" s="3"/>
     </row>
     <row r="391" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z391" s="2"/>
+      <c r="Z391" s="3"/>
     </row>
     <row r="392" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z392" s="2"/>
+      <c r="Z392" s="3"/>
     </row>
     <row r="393" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z393" s="2"/>
+      <c r="Z393" s="3"/>
     </row>
     <row r="394" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z394" s="2"/>
+      <c r="Z394" s="3"/>
     </row>
     <row r="395" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z395" s="2"/>
+      <c r="Z395" s="3"/>
     </row>
     <row r="396" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z396" s="2"/>
+      <c r="Z396" s="3"/>
     </row>
     <row r="397" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z397" s="2"/>
+      <c r="Z397" s="3"/>
     </row>
     <row r="398" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z398" s="2"/>
+      <c r="Z398" s="3"/>
     </row>
     <row r="399" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z399" s="2"/>
+      <c r="Z399" s="3"/>
     </row>
     <row r="400" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z400" s="2"/>
+      <c r="Z400" s="3"/>
     </row>
     <row r="401" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z401" s="2"/>
+      <c r="Z401" s="3"/>
     </row>
     <row r="402" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z402" s="2"/>
+      <c r="Z402" s="3"/>
     </row>
     <row r="403" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z403" s="2"/>
+      <c r="Z403" s="3"/>
     </row>
     <row r="404" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z404" s="2"/>
+      <c r="Z404" s="3"/>
     </row>
     <row r="405" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z405" s="2"/>
+      <c r="Z405" s="3"/>
     </row>
     <row r="406" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z406" s="2"/>
+      <c r="Z406" s="3"/>
     </row>
     <row r="407" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z407" s="2"/>
+      <c r="Z407" s="3"/>
     </row>
     <row r="408" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z408" s="2"/>
+      <c r="Z408" s="3"/>
     </row>
     <row r="409" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z409" s="2"/>
+      <c r="Z409" s="3"/>
     </row>
     <row r="410" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z410" s="2"/>
+      <c r="Z410" s="3"/>
     </row>
     <row r="411" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z411" s="2"/>
+      <c r="Z411" s="3"/>
     </row>
     <row r="412" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z412" s="2"/>
+      <c r="Z412" s="3"/>
     </row>
     <row r="413" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z413" s="2"/>
+      <c r="Z413" s="3"/>
     </row>
     <row r="414" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z414" s="2"/>
+      <c r="Z414" s="3"/>
     </row>
     <row r="415" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z415" s="2"/>
+      <c r="Z415" s="3"/>
     </row>
     <row r="416" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z416" s="2"/>
+      <c r="Z416" s="3"/>
     </row>
     <row r="417" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z417" s="2"/>
+      <c r="Z417" s="3"/>
     </row>
     <row r="418" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z418" s="2"/>
+      <c r="Z418" s="3"/>
     </row>
     <row r="419" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z419" s="2"/>
+      <c r="Z419" s="3"/>
     </row>
     <row r="420" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z420" s="2"/>
+      <c r="Z420" s="3"/>
     </row>
     <row r="421" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z421" s="2"/>
+      <c r="Z421" s="3"/>
     </row>
     <row r="422" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z422" s="2"/>
+      <c r="Z422" s="3"/>
     </row>
     <row r="423" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z423" s="2"/>
+      <c r="Z423" s="3"/>
     </row>
     <row r="424" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z424" s="2"/>
+      <c r="Z424" s="3"/>
     </row>
     <row r="425" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z425" s="2"/>
+      <c r="Z425" s="3"/>
     </row>
     <row r="426" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z426" s="2"/>
+      <c r="Z426" s="3"/>
     </row>
     <row r="427" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z427" s="2"/>
+      <c r="Z427" s="3"/>
     </row>
     <row r="428" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z428" s="2"/>
+      <c r="Z428" s="3"/>
     </row>
     <row r="429" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z429" s="2"/>
+      <c r="Z429" s="3"/>
     </row>
     <row r="430" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z430" s="2"/>
+      <c r="Z430" s="3"/>
     </row>
     <row r="431" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z431" s="2"/>
+      <c r="Z431" s="3"/>
     </row>
     <row r="432" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z432" s="2"/>
+      <c r="Z432" s="3"/>
     </row>
     <row r="433" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z433" s="2"/>
+      <c r="Z433" s="3"/>
     </row>
     <row r="434" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z434" s="2"/>
+      <c r="Z434" s="3"/>
     </row>
     <row r="435" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z435" s="2"/>
+      <c r="Z435" s="3"/>
     </row>
     <row r="436" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z436" s="2"/>
+      <c r="Z436" s="3"/>
     </row>
     <row r="437" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z437" s="2"/>
+      <c r="Z437" s="3"/>
     </row>
     <row r="438" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z438" s="2"/>
+      <c r="Z438" s="3"/>
     </row>
     <row r="439" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z439" s="2"/>
+      <c r="Z439" s="3"/>
     </row>
     <row r="440" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z440" s="2"/>
+      <c r="Z440" s="3"/>
     </row>
     <row r="441" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z441" s="2"/>
+      <c r="Z441" s="3"/>
     </row>
     <row r="442" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z442" s="2"/>
+      <c r="Z442" s="3"/>
     </row>
     <row r="443" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z443" s="2"/>
+      <c r="Z443" s="3"/>
     </row>
     <row r="444" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z444" s="2"/>
+      <c r="Z444" s="3"/>
     </row>
     <row r="445" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z445" s="2"/>
+      <c r="Z445" s="3"/>
     </row>
     <row r="446" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z446" s="2"/>
+      <c r="Z446" s="3"/>
     </row>
     <row r="447" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z447" s="2"/>
+      <c r="Z447" s="3"/>
     </row>
     <row r="448" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z448" s="2"/>
+      <c r="Z448" s="3"/>
     </row>
     <row r="449" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z449" s="2"/>
+      <c r="Z449" s="3"/>
     </row>
     <row r="450" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z450" s="2"/>
+      <c r="Z450" s="3"/>
     </row>
     <row r="451" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z451" s="2"/>
+      <c r="Z451" s="3"/>
     </row>
     <row r="452" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z452" s="2"/>
+      <c r="Z452" s="3"/>
     </row>
     <row r="453" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z453" s="2"/>
+      <c r="Z453" s="3"/>
     </row>
     <row r="454" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z454" s="2"/>
+      <c r="Z454" s="3"/>
     </row>
     <row r="455" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z455" s="2"/>
+      <c r="Z455" s="3"/>
     </row>
     <row r="456" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z456" s="2"/>
+      <c r="Z456" s="3"/>
     </row>
     <row r="457" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z457" s="2"/>
+      <c r="Z457" s="3"/>
     </row>
     <row r="458" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z458" s="2"/>
+      <c r="Z458" s="3"/>
     </row>
     <row r="459" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z459" s="2"/>
+      <c r="Z459" s="3"/>
     </row>
     <row r="460" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z460" s="2"/>
+      <c r="Z460" s="3"/>
     </row>
     <row r="461" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z461" s="2"/>
+      <c r="Z461" s="3"/>
     </row>
     <row r="462" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z462" s="2"/>
+      <c r="Z462" s="3"/>
     </row>
     <row r="463" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z463" s="2"/>
+      <c r="Z463" s="3"/>
     </row>
     <row r="464" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z464" s="2"/>
+      <c r="Z464" s="3"/>
     </row>
     <row r="465" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z465" s="2"/>
+      <c r="Z465" s="3"/>
     </row>
     <row r="466" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z466" s="2"/>
+      <c r="Z466" s="3"/>
     </row>
     <row r="467" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z467" s="2"/>
+      <c r="Z467" s="3"/>
     </row>
     <row r="468" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z468" s="2"/>
+      <c r="Z468" s="3"/>
     </row>
     <row r="469" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z469" s="2"/>
+      <c r="Z469" s="3"/>
     </row>
     <row r="470" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z470" s="2"/>
+      <c r="Z470" s="3"/>
     </row>
     <row r="471" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z471" s="2"/>
+      <c r="Z471" s="3"/>
     </row>
     <row r="472" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z472" s="2"/>
+      <c r="Z472" s="3"/>
     </row>
     <row r="473" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z473" s="2"/>
+      <c r="Z473" s="3"/>
     </row>
     <row r="474" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z474" s="2"/>
+      <c r="Z474" s="3"/>
     </row>
     <row r="475" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z475" s="2"/>
+      <c r="Z475" s="3"/>
     </row>
     <row r="476" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z476" s="2"/>
+      <c r="Z476" s="3"/>
     </row>
     <row r="477" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z477" s="2"/>
+      <c r="Z477" s="3"/>
     </row>
     <row r="478" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z478" s="2"/>
+      <c r="Z478" s="3"/>
     </row>
     <row r="479" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z479" s="2"/>
+      <c r="Z479" s="3"/>
     </row>
     <row r="480" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z480" s="2"/>
+      <c r="Z480" s="3"/>
     </row>
     <row r="481" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z481" s="2"/>
+      <c r="Z481" s="3"/>
     </row>
     <row r="482" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z482" s="2"/>
+      <c r="Z482" s="3"/>
     </row>
     <row r="483" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z483" s="2"/>
+      <c r="Z483" s="3"/>
     </row>
     <row r="484" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z484" s="2"/>
+      <c r="Z484" s="3"/>
     </row>
     <row r="485" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z485" s="2"/>
+      <c r="Z485" s="3"/>
     </row>
     <row r="486" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z486" s="2"/>
+      <c r="Z486" s="3"/>
     </row>
     <row r="487" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z487" s="2"/>
+      <c r="Z487" s="3"/>
     </row>
     <row r="488" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z488" s="2"/>
+      <c r="Z488" s="3"/>
     </row>
     <row r="489" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z489" s="2"/>
+      <c r="Z489" s="3"/>
     </row>
     <row r="490" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z490" s="2"/>
+      <c r="Z490" s="3"/>
     </row>
     <row r="491" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z491" s="2"/>
+      <c r="Z491" s="3"/>
     </row>
     <row r="492" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z492" s="2"/>
+      <c r="Z492" s="3"/>
     </row>
     <row r="493" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z493" s="2"/>
+      <c r="Z493" s="3"/>
     </row>
     <row r="494" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z494" s="2"/>
+      <c r="Z494" s="3"/>
     </row>
     <row r="495" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z495" s="2"/>
+      <c r="Z495" s="3"/>
     </row>
     <row r="496" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z496" s="2"/>
+      <c r="Z496" s="3"/>
     </row>
     <row r="497" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z497" s="2"/>
+      <c r="Z497" s="3"/>
     </row>
     <row r="498" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z498" s="2"/>
+      <c r="Z498" s="3"/>
     </row>
     <row r="499" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z499" s="2"/>
+      <c r="Z499" s="3"/>
     </row>
     <row r="500" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z500" s="2"/>
+      <c r="Z500" s="3"/>
     </row>
     <row r="501" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z501" s="2"/>
+      <c r="Z501" s="3"/>
     </row>
     <row r="502" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z502" s="2"/>
+      <c r="Z502" s="3"/>
     </row>
     <row r="503" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z503" s="2"/>
+      <c r="Z503" s="3"/>
     </row>
     <row r="504" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z504" s="2"/>
+      <c r="Z504" s="3"/>
     </row>
     <row r="505" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z505" s="2"/>
+      <c r="Z505" s="3"/>
     </row>
     <row r="506" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z506" s="2"/>
+      <c r="Z506" s="3"/>
     </row>
     <row r="507" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z507" s="2"/>
+      <c r="Z507" s="3"/>
     </row>
     <row r="508" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z508" s="2"/>
+      <c r="Z508" s="3"/>
     </row>
     <row r="509" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z509" s="2"/>
+      <c r="Z509" s="3"/>
     </row>
     <row r="510" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z510" s="2"/>
+      <c r="Z510" s="3"/>
     </row>
     <row r="511" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z511" s="2"/>
+      <c r="Z511" s="3"/>
     </row>
     <row r="512" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z512" s="2"/>
+      <c r="Z512" s="3"/>
     </row>
     <row r="513" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z513" s="2"/>
+      <c r="Z513" s="3"/>
     </row>
     <row r="514" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z514" s="2"/>
+      <c r="Z514" s="3"/>
     </row>
     <row r="515" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z515" s="2"/>
+      <c r="Z515" s="3"/>
     </row>
     <row r="516" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z516" s="2"/>
+      <c r="Z516" s="3"/>
     </row>
     <row r="517" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z517" s="2"/>
+      <c r="Z517" s="3"/>
     </row>
     <row r="518" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z518" s="2"/>
+      <c r="Z518" s="3"/>
     </row>
     <row r="519" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z519" s="2"/>
+      <c r="Z519" s="3"/>
     </row>
     <row r="520" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z520" s="2"/>
+      <c r="Z520" s="3"/>
     </row>
     <row r="521" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z521" s="2"/>
+      <c r="Z521" s="3"/>
     </row>
     <row r="522" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z522" s="2"/>
+      <c r="Z522" s="3"/>
     </row>
     <row r="523" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z523" s="2"/>
+      <c r="Z523" s="3"/>
     </row>
     <row r="524" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z524" s="2"/>
+      <c r="Z524" s="3"/>
     </row>
     <row r="525" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z525" s="2"/>
+      <c r="Z525" s="3"/>
     </row>
     <row r="526" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z526" s="2"/>
+      <c r="Z526" s="3"/>
     </row>
     <row r="527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z527" s="2"/>
+      <c r="Z527" s="3"/>
     </row>
     <row r="528" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z528" s="2"/>
+      <c r="Z528" s="3"/>
     </row>
     <row r="529" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z529" s="2"/>
+      <c r="Z529" s="3"/>
     </row>
     <row r="530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z530" s="2"/>
+      <c r="Z530" s="3"/>
     </row>
     <row r="531" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z531" s="2"/>
+      <c r="Z531" s="3"/>
     </row>
     <row r="532" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z532" s="2"/>
+      <c r="Z532" s="3"/>
     </row>
     <row r="533" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z533" s="2"/>
+      <c r="Z533" s="3"/>
     </row>
     <row r="534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z534" s="2"/>
+      <c r="Z534" s="3"/>
     </row>
     <row r="535" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z535" s="2"/>
+      <c r="Z535" s="3"/>
     </row>
     <row r="536" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z536" s="2"/>
+      <c r="Z536" s="3"/>
     </row>
     <row r="537" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z537" s="2"/>
+      <c r="Z537" s="3"/>
     </row>
     <row r="538" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z538" s="2"/>
+      <c r="Z538" s="3"/>
     </row>
     <row r="539" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z539" s="2"/>
+      <c r="Z539" s="3"/>
     </row>
     <row r="540" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z540" s="2"/>
+      <c r="Z540" s="3"/>
     </row>
     <row r="541" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z541" s="2"/>
+      <c r="Z541" s="3"/>
     </row>
     <row r="542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z542" s="2"/>
+      <c r="Z542" s="3"/>
     </row>
     <row r="543" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z543" s="2"/>
+      <c r="Z543" s="3"/>
     </row>
     <row r="544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z544" s="2"/>
+      <c r="Z544" s="3"/>
     </row>
     <row r="545" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z545" s="2"/>
+      <c r="Z545" s="3"/>
     </row>
     <row r="546" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z546" s="2"/>
+      <c r="Z546" s="3"/>
     </row>
     <row r="547" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z547" s="2"/>
+      <c r="Z547" s="3"/>
     </row>
     <row r="548" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z548" s="2"/>
+      <c r="Z548" s="3"/>
     </row>
     <row r="549" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z549" s="2"/>
+      <c r="Z549" s="3"/>
     </row>
     <row r="550" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z550" s="2"/>
+      <c r="Z550" s="3"/>
     </row>
     <row r="551" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z551" s="2"/>
+      <c r="Z551" s="3"/>
     </row>
     <row r="552" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z552" s="2"/>
+      <c r="Z552" s="3"/>
     </row>
     <row r="553" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z553" s="2"/>
+      <c r="Z553" s="3"/>
     </row>
     <row r="554" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z554" s="2"/>
+      <c r="Z554" s="3"/>
     </row>
     <row r="555" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z555" s="2"/>
+      <c r="Z555" s="3"/>
     </row>
     <row r="556" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z556" s="2"/>
+      <c r="Z556" s="3"/>
     </row>
     <row r="557" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z557" s="2"/>
+      <c r="Z557" s="3"/>
     </row>
     <row r="558" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z558" s="2"/>
+      <c r="Z558" s="3"/>
     </row>
     <row r="559" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z559" s="2"/>
+      <c r="Z559" s="3"/>
     </row>
     <row r="560" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z560" s="2"/>
+      <c r="Z560" s="3"/>
     </row>
     <row r="561" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z561" s="2"/>
+      <c r="Z561" s="3"/>
     </row>
     <row r="562" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z562" s="2"/>
+      <c r="Z562" s="3"/>
     </row>
     <row r="563" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z563" s="2"/>
+      <c r="Z563" s="3"/>
     </row>
     <row r="564" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z564" s="2"/>
+      <c r="Z564" s="3"/>
     </row>
     <row r="565" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z565" s="2"/>
+      <c r="Z565" s="3"/>
     </row>
     <row r="566" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z566" s="2"/>
+      <c r="Z566" s="3"/>
     </row>
     <row r="567" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z567" s="2"/>
+      <c r="Z567" s="3"/>
     </row>
     <row r="568" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z568" s="2"/>
+      <c r="Z568" s="3"/>
     </row>
     <row r="569" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z569" s="2"/>
+      <c r="Z569" s="3"/>
     </row>
     <row r="570" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z570" s="2"/>
+      <c r="Z570" s="3"/>
     </row>
     <row r="571" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z571" s="2"/>
+      <c r="Z571" s="3"/>
     </row>
     <row r="572" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z572" s="2"/>
+      <c r="Z572" s="3"/>
     </row>
     <row r="573" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z573" s="2"/>
+      <c r="Z573" s="3"/>
     </row>
     <row r="574" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z574" s="2"/>
+      <c r="Z574" s="3"/>
     </row>
     <row r="575" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z575" s="2"/>
+      <c r="Z575" s="3"/>
     </row>
     <row r="576" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z576" s="2"/>
+      <c r="Z576" s="3"/>
     </row>
     <row r="577" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z577" s="2"/>
+      <c r="Z577" s="3"/>
     </row>
     <row r="578" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z578" s="2"/>
+      <c r="Z578" s="3"/>
     </row>
     <row r="579" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z579" s="2"/>
+      <c r="Z579" s="3"/>
     </row>
     <row r="580" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z580" s="2"/>
+      <c r="Z580" s="3"/>
     </row>
     <row r="581" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z581" s="2"/>
+      <c r="Z581" s="3"/>
     </row>
     <row r="582" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z582" s="2"/>
+      <c r="Z582" s="3"/>
     </row>
     <row r="583" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z583" s="2"/>
+      <c r="Z583" s="3"/>
     </row>
     <row r="584" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z584" s="2"/>
+      <c r="Z584" s="3"/>
     </row>
     <row r="585" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z585" s="2"/>
+      <c r="Z585" s="3"/>
     </row>
     <row r="586" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z586" s="2"/>
+      <c r="Z586" s="3"/>
     </row>
     <row r="587" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z587" s="2"/>
+      <c r="Z587" s="3"/>
     </row>
     <row r="588" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z588" s="2"/>
+      <c r="Z588" s="3"/>
     </row>
     <row r="589" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z589" s="2"/>
+      <c r="Z589" s="3"/>
     </row>
     <row r="590" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z590" s="2"/>
+      <c r="Z590" s="3"/>
     </row>
     <row r="591" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z591" s="2"/>
+      <c r="Z591" s="3"/>
     </row>
     <row r="592" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z592" s="2"/>
+      <c r="Z592" s="3"/>
     </row>
     <row r="593" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z593" s="2"/>
+      <c r="Z593" s="3"/>
     </row>
     <row r="594" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z594" s="2"/>
+      <c r="Z594" s="3"/>
     </row>
     <row r="595" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z595" s="2"/>
+      <c r="Z595" s="3"/>
     </row>
     <row r="596" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z596" s="2"/>
+      <c r="Z596" s="3"/>
     </row>
     <row r="597" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z597" s="2"/>
+      <c r="Z597" s="3"/>
     </row>
     <row r="598" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z598" s="2"/>
+      <c r="Z598" s="3"/>
     </row>
     <row r="599" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z599" s="2"/>
+      <c r="Z599" s="3"/>
     </row>
     <row r="600" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z600" s="2"/>
+      <c r="Z600" s="3"/>
     </row>
     <row r="601" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z601" s="2"/>
+      <c r="Z601" s="3"/>
     </row>
     <row r="602" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z602" s="2"/>
+      <c r="Z602" s="3"/>
     </row>
     <row r="603" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z603" s="2"/>
+      <c r="Z603" s="3"/>
     </row>
     <row r="604" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z604" s="2"/>
+      <c r="Z604" s="3"/>
     </row>
     <row r="605" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z605" s="2"/>
+      <c r="Z605" s="3"/>
     </row>
     <row r="606" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z606" s="2"/>
+      <c r="Z606" s="3"/>
     </row>
     <row r="607" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z607" s="2"/>
+      <c r="Z607" s="3"/>
     </row>
     <row r="608" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z608" s="2"/>
+      <c r="Z608" s="3"/>
     </row>
     <row r="609" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z609" s="2"/>
+      <c r="Z609" s="3"/>
     </row>
     <row r="610" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z610" s="2"/>
+      <c r="Z610" s="3"/>
     </row>
     <row r="611" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z611" s="2"/>
+      <c r="Z611" s="3"/>
     </row>
     <row r="612" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z612" s="2"/>
+      <c r="Z612" s="3"/>
     </row>
     <row r="613" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z613" s="2"/>
+      <c r="Z613" s="3"/>
     </row>
     <row r="614" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z614" s="2"/>
+      <c r="Z614" s="3"/>
     </row>
     <row r="615" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z615" s="2"/>
+      <c r="Z615" s="3"/>
     </row>
     <row r="616" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z616" s="2"/>
+      <c r="Z616" s="3"/>
     </row>
     <row r="617" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z617" s="2"/>
+      <c r="Z617" s="3"/>
     </row>
     <row r="618" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z618" s="2"/>
+      <c r="Z618" s="3"/>
     </row>
     <row r="619" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z619" s="2"/>
+      <c r="Z619" s="3"/>
     </row>
     <row r="620" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z620" s="2"/>
+      <c r="Z620" s="3"/>
     </row>
     <row r="621" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z621" s="2"/>
+      <c r="Z621" s="3"/>
     </row>
     <row r="622" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z622" s="2"/>
+      <c r="Z622" s="3"/>
     </row>
     <row r="623" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z623" s="2"/>
+      <c r="Z623" s="3"/>
     </row>
     <row r="624" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z624" s="2"/>
+      <c r="Z624" s="3"/>
     </row>
     <row r="625" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z625" s="2"/>
+      <c r="Z625" s="3"/>
     </row>
     <row r="626" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z626" s="2"/>
+      <c r="Z626" s="3"/>
     </row>
     <row r="627" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z627" s="2"/>
+      <c r="Z627" s="3"/>
     </row>
     <row r="628" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z628" s="2"/>
+      <c r="Z628" s="3"/>
     </row>
     <row r="629" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z629" s="2"/>
+      <c r="Z629" s="3"/>
     </row>
     <row r="630" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z630" s="2"/>
+      <c r="Z630" s="3"/>
     </row>
     <row r="631" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z631" s="2"/>
+      <c r="Z631" s="3"/>
     </row>
     <row r="632" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z632" s="2"/>
+      <c r="Z632" s="3"/>
     </row>
     <row r="633" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z633" s="2"/>
+      <c r="Z633" s="3"/>
     </row>
     <row r="634" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z634" s="2"/>
+      <c r="Z634" s="3"/>
     </row>
     <row r="635" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z635" s="2"/>
+      <c r="Z635" s="3"/>
     </row>
     <row r="636" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z636" s="2"/>
+      <c r="Z636" s="3"/>
     </row>
     <row r="637" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z637" s="2"/>
+      <c r="Z637" s="3"/>
     </row>
     <row r="638" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z638" s="2"/>
+      <c r="Z638" s="3"/>
     </row>
     <row r="639" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z639" s="2"/>
+      <c r="Z639" s="3"/>
     </row>
     <row r="640" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z640" s="2"/>
+      <c r="Z640" s="3"/>
     </row>
     <row r="641" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z641" s="2"/>
+      <c r="Z641" s="3"/>
     </row>
     <row r="642" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z642" s="2"/>
+      <c r="Z642" s="3"/>
     </row>
     <row r="643" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z643" s="2"/>
+      <c r="Z643" s="3"/>
     </row>
     <row r="644" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z644" s="2"/>
+      <c r="Z644" s="3"/>
     </row>
     <row r="645" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z645" s="2"/>
+      <c r="Z645" s="3"/>
     </row>
     <row r="646" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z646" s="2"/>
+      <c r="Z646" s="3"/>
     </row>
     <row r="647" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z647" s="2"/>
+      <c r="Z647" s="3"/>
     </row>
     <row r="648" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z648" s="2"/>
+      <c r="Z648" s="3"/>
     </row>
     <row r="649" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z649" s="2"/>
+      <c r="Z649" s="3"/>
     </row>
     <row r="650" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z650" s="2"/>
+      <c r="Z650" s="3"/>
     </row>
     <row r="651" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z651" s="2"/>
+      <c r="Z651" s="3"/>
     </row>
     <row r="652" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z652" s="2"/>
+      <c r="Z652" s="3"/>
     </row>
     <row r="653" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z653" s="2"/>
+      <c r="Z653" s="3"/>
     </row>
     <row r="654" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z654" s="2"/>
+      <c r="Z654" s="3"/>
     </row>
     <row r="655" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z655" s="2"/>
+      <c r="Z655" s="3"/>
     </row>
     <row r="656" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z656" s="2"/>
+      <c r="Z656" s="3"/>
     </row>
     <row r="657" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z657" s="2"/>
+      <c r="Z657" s="3"/>
     </row>
     <row r="658" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z658" s="2"/>
+      <c r="Z658" s="3"/>
     </row>
     <row r="659" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z659" s="2"/>
+      <c r="Z659" s="3"/>
     </row>
     <row r="660" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z660" s="2"/>
+      <c r="Z660" s="3"/>
     </row>
     <row r="661" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z661" s="2"/>
+      <c r="Z661" s="3"/>
     </row>
     <row r="662" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z662" s="2"/>
+      <c r="Z662" s="3"/>
     </row>
     <row r="663" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z663" s="2"/>
+      <c r="Z663" s="3"/>
     </row>
     <row r="664" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z664" s="2"/>
+      <c r="Z664" s="3"/>
     </row>
     <row r="665" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z665" s="2"/>
+      <c r="Z665" s="3"/>
     </row>
     <row r="666" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z666" s="2"/>
+      <c r="Z666" s="3"/>
     </row>
     <row r="667" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z667" s="2"/>
+      <c r="Z667" s="3"/>
     </row>
     <row r="668" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z668" s="2"/>
+      <c r="Z668" s="3"/>
     </row>
     <row r="669" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z669" s="2"/>
+      <c r="Z669" s="3"/>
     </row>
     <row r="670" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z670" s="2"/>
+      <c r="Z670" s="3"/>
     </row>
     <row r="671" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z671" s="2"/>
+      <c r="Z671" s="3"/>
     </row>
     <row r="672" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z672" s="2"/>
+      <c r="Z672" s="3"/>
     </row>
     <row r="673" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z673" s="2"/>
+      <c r="Z673" s="3"/>
     </row>
     <row r="674" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z674" s="2"/>
+      <c r="Z674" s="3"/>
     </row>
     <row r="675" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z675" s="2"/>
+      <c r="Z675" s="3"/>
     </row>
     <row r="676" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z676" s="2"/>
+      <c r="Z676" s="3"/>
     </row>
     <row r="677" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z677" s="2"/>
+      <c r="Z677" s="3"/>
     </row>
     <row r="678" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z678" s="2"/>
+      <c r="Z678" s="3"/>
     </row>
     <row r="679" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z679" s="2"/>
+      <c r="Z679" s="3"/>
     </row>
     <row r="680" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z680" s="2"/>
+      <c r="Z680" s="3"/>
     </row>
     <row r="681" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z681" s="2"/>
+      <c r="Z681" s="3"/>
     </row>
     <row r="682" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z682" s="2"/>
+      <c r="Z682" s="3"/>
     </row>
     <row r="683" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z683" s="2"/>
+      <c r="Z683" s="3"/>
     </row>
     <row r="684" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z684" s="2"/>
+      <c r="Z684" s="3"/>
     </row>
     <row r="685" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z685" s="2"/>
+      <c r="Z685" s="3"/>
     </row>
     <row r="686" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z686" s="2"/>
+      <c r="Z686" s="3"/>
     </row>
     <row r="687" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z687" s="2"/>
+      <c r="Z687" s="3"/>
     </row>
     <row r="688" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z688" s="2"/>
+      <c r="Z688" s="3"/>
     </row>
     <row r="689" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z689" s="2"/>
+      <c r="Z689" s="3"/>
     </row>
     <row r="690" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z690" s="2"/>
+      <c r="Z690" s="3"/>
     </row>
     <row r="691" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z691" s="2"/>
+      <c r="Z691" s="3"/>
     </row>
     <row r="692" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z692" s="2"/>
+      <c r="Z692" s="3"/>
     </row>
     <row r="693" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z693" s="2"/>
+      <c r="Z693" s="3"/>
     </row>
     <row r="694" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z694" s="2"/>
+      <c r="Z694" s="3"/>
     </row>
     <row r="695" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z695" s="2"/>
+      <c r="Z695" s="3"/>
     </row>
     <row r="696" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z696" s="2"/>
+      <c r="Z696" s="3"/>
     </row>
     <row r="697" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z697" s="2"/>
+      <c r="Z697" s="3"/>
     </row>
     <row r="698" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z698" s="2"/>
+      <c r="Z698" s="3"/>
     </row>
     <row r="699" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z699" s="2"/>
+      <c r="Z699" s="3"/>
     </row>
     <row r="700" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z700" s="2"/>
+      <c r="Z700" s="3"/>
     </row>
     <row r="701" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z701" s="2"/>
+      <c r="Z701" s="3"/>
     </row>
     <row r="702" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z702" s="2"/>
+      <c r="Z702" s="3"/>
     </row>
     <row r="703" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z703" s="2"/>
+      <c r="Z703" s="3"/>
     </row>
     <row r="704" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z704" s="2"/>
+      <c r="Z704" s="3"/>
     </row>
     <row r="705" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z705" s="2"/>
+      <c r="Z705" s="3"/>
     </row>
     <row r="706" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z706" s="2"/>
+      <c r="Z706" s="3"/>
     </row>
     <row r="707" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z707" s="2"/>
+      <c r="Z707" s="3"/>
     </row>
     <row r="708" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z708" s="2"/>
+      <c r="Z708" s="3"/>
     </row>
     <row r="709" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z709" s="2"/>
+      <c r="Z709" s="3"/>
     </row>
     <row r="710" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z710" s="2"/>
+      <c r="Z710" s="3"/>
     </row>
     <row r="711" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z711" s="2"/>
+      <c r="Z711" s="3"/>
     </row>
     <row r="712" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z712" s="2"/>
+      <c r="Z712" s="3"/>
     </row>
     <row r="713" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z713" s="2"/>
+      <c r="Z713" s="3"/>
     </row>
     <row r="714" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z714" s="2"/>
+      <c r="Z714" s="3"/>
     </row>
     <row r="715" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z715" s="2"/>
+      <c r="Z715" s="3"/>
     </row>
     <row r="716" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z716" s="2"/>
+      <c r="Z716" s="3"/>
     </row>
     <row r="717" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z717" s="2"/>
+      <c r="Z717" s="3"/>
     </row>
     <row r="718" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z718" s="2"/>
+      <c r="Z718" s="3"/>
     </row>
     <row r="719" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z719" s="2"/>
+      <c r="Z719" s="3"/>
     </row>
     <row r="720" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z720" s="2"/>
+      <c r="Z720" s="3"/>
     </row>
     <row r="721" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z721" s="2"/>
+      <c r="Z721" s="3"/>
     </row>
     <row r="722" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z722" s="2"/>
+      <c r="Z722" s="3"/>
     </row>
     <row r="723" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z723" s="2"/>
+      <c r="Z723" s="3"/>
     </row>
     <row r="724" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z724" s="2"/>
+      <c r="Z724" s="3"/>
     </row>
     <row r="725" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z725" s="2"/>
+      <c r="Z725" s="3"/>
     </row>
     <row r="726" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z726" s="2"/>
+      <c r="Z726" s="3"/>
     </row>
     <row r="727" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z727" s="2"/>
+      <c r="Z727" s="3"/>
     </row>
     <row r="728" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z728" s="2"/>
+      <c r="Z728" s="3"/>
     </row>
     <row r="729" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z729" s="2"/>
+      <c r="Z729" s="3"/>
     </row>
     <row r="730" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z730" s="2"/>
+      <c r="Z730" s="3"/>
     </row>
     <row r="731" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z731" s="2"/>
+      <c r="Z731" s="3"/>
     </row>
     <row r="732" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z732" s="2"/>
+      <c r="Z732" s="3"/>
     </row>
     <row r="733" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z733" s="2"/>
+      <c r="Z733" s="3"/>
     </row>
     <row r="734" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z734" s="2"/>
+      <c r="Z734" s="3"/>
     </row>
     <row r="735" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z735" s="2"/>
+      <c r="Z735" s="3"/>
     </row>
     <row r="736" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z736" s="2"/>
+      <c r="Z736" s="3"/>
     </row>
     <row r="737" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z737" s="2"/>
+      <c r="Z737" s="3"/>
     </row>
     <row r="738" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z738" s="2"/>
+      <c r="Z738" s="3"/>
     </row>
     <row r="739" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z739" s="2"/>
+      <c r="Z739" s="3"/>
     </row>
     <row r="740" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z740" s="2"/>
+      <c r="Z740" s="3"/>
     </row>
     <row r="741" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z741" s="2"/>
+      <c r="Z741" s="3"/>
     </row>
     <row r="742" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z742" s="2"/>
+      <c r="Z742" s="3"/>
     </row>
     <row r="743" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z743" s="2"/>
+      <c r="Z743" s="3"/>
     </row>
     <row r="744" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z744" s="2"/>
+      <c r="Z744" s="3"/>
     </row>
     <row r="745" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z745" s="2"/>
+      <c r="Z745" s="3"/>
     </row>
     <row r="746" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z746" s="2"/>
+      <c r="Z746" s="3"/>
     </row>
     <row r="747" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z747" s="2"/>
+      <c r="Z747" s="3"/>
     </row>
     <row r="748" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z748" s="2"/>
+      <c r="Z748" s="3"/>
     </row>
     <row r="749" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z749" s="2"/>
+      <c r="Z749" s="3"/>
     </row>
     <row r="750" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z750" s="2"/>
+      <c r="Z750" s="3"/>
     </row>
     <row r="751" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z751" s="2"/>
+      <c r="Z751" s="3"/>
     </row>
     <row r="752" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z752" s="2"/>
+      <c r="Z752" s="3"/>
     </row>
     <row r="753" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z753" s="2"/>
+      <c r="Z753" s="3"/>
     </row>
     <row r="754" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z754" s="2"/>
+      <c r="Z754" s="3"/>
     </row>
     <row r="755" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z755" s="2"/>
+      <c r="Z755" s="3"/>
     </row>
     <row r="756" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z756" s="2"/>
+      <c r="Z756" s="3"/>
     </row>
     <row r="757" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z757" s="2"/>
+      <c r="Z757" s="3"/>
     </row>
     <row r="758" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z758" s="2"/>
+      <c r="Z758" s="3"/>
     </row>
     <row r="759" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z759" s="2"/>
+      <c r="Z759" s="3"/>
     </row>
     <row r="760" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z760" s="2"/>
+      <c r="Z760" s="3"/>
     </row>
     <row r="761" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z761" s="2"/>
+      <c r="Z761" s="3"/>
     </row>
     <row r="762" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z762" s="2"/>
+      <c r="Z762" s="3"/>
     </row>
     <row r="763" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z763" s="2"/>
+      <c r="Z763" s="3"/>
     </row>
     <row r="764" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z764" s="2"/>
+      <c r="Z764" s="3"/>
     </row>
     <row r="765" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z765" s="2"/>
+      <c r="Z765" s="3"/>
     </row>
     <row r="766" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z766" s="2"/>
+      <c r="Z766" s="3"/>
     </row>
     <row r="767" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z767" s="2"/>
+      <c r="Z767" s="3"/>
     </row>
     <row r="768" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z768" s="2"/>
+      <c r="Z768" s="3"/>
     </row>
     <row r="769" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z769" s="2"/>
+      <c r="Z769" s="3"/>
     </row>
     <row r="770" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z770" s="2"/>
+      <c r="Z770" s="3"/>
     </row>
     <row r="771" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z771" s="2"/>
+      <c r="Z771" s="3"/>
     </row>
     <row r="772" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z772" s="2"/>
+      <c r="Z772" s="3"/>
     </row>
     <row r="773" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z773" s="2"/>
+      <c r="Z773" s="3"/>
     </row>
     <row r="774" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z774" s="2"/>
+      <c r="Z774" s="3"/>
     </row>
     <row r="775" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z775" s="2"/>
+      <c r="Z775" s="3"/>
     </row>
     <row r="776" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z776" s="2"/>
+      <c r="Z776" s="3"/>
     </row>
     <row r="777" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z777" s="2"/>
+      <c r="Z777" s="3"/>
     </row>
     <row r="778" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z778" s="2"/>
+      <c r="Z778" s="3"/>
     </row>
     <row r="779" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z779" s="2"/>
+      <c r="Z779" s="3"/>
     </row>
     <row r="780" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z780" s="2"/>
+      <c r="Z780" s="3"/>
     </row>
     <row r="781" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z781" s="2"/>
+      <c r="Z781" s="3"/>
     </row>
     <row r="782" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z782" s="2"/>
+      <c r="Z782" s="3"/>
     </row>
     <row r="783" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z783" s="2"/>
+      <c r="Z783" s="3"/>
     </row>
     <row r="784" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z784" s="2"/>
+      <c r="Z784" s="3"/>
     </row>
     <row r="785" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z785" s="2"/>
+      <c r="Z785" s="3"/>
     </row>
     <row r="786" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z786" s="2"/>
+      <c r="Z786" s="3"/>
     </row>
     <row r="787" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z787" s="2"/>
+      <c r="Z787" s="3"/>
     </row>
     <row r="788" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z788" s="2"/>
+      <c r="Z788" s="3"/>
     </row>
     <row r="789" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z789" s="2"/>
+      <c r="Z789" s="3"/>
     </row>
     <row r="790" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z790" s="2"/>
+      <c r="Z790" s="3"/>
     </row>
     <row r="791" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z791" s="2"/>
+      <c r="Z791" s="3"/>
     </row>
     <row r="792" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z792" s="2"/>
+      <c r="Z792" s="3"/>
     </row>
     <row r="793" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z793" s="2"/>
+      <c r="Z793" s="3"/>
     </row>
     <row r="794" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z794" s="2"/>
+      <c r="Z794" s="3"/>
     </row>
     <row r="795" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z795" s="2"/>
+      <c r="Z795" s="3"/>
     </row>
     <row r="796" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z796" s="2"/>
+      <c r="Z796" s="3"/>
     </row>
     <row r="797" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z797" s="2"/>
+      <c r="Z797" s="3"/>
     </row>
     <row r="798" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z798" s="2"/>
+      <c r="Z798" s="3"/>
     </row>
     <row r="799" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z799" s="2"/>
+      <c r="Z799" s="3"/>
     </row>
     <row r="800" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z800" s="2"/>
+      <c r="Z800" s="3"/>
     </row>
     <row r="801" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z801" s="2"/>
+      <c r="Z801" s="3"/>
     </row>
     <row r="802" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z802" s="2"/>
+      <c r="Z802" s="3"/>
     </row>
     <row r="803" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z803" s="2"/>
+      <c r="Z803" s="3"/>
     </row>
     <row r="804" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z804" s="2"/>
+      <c r="Z804" s="3"/>
     </row>
     <row r="805" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z805" s="2"/>
+      <c r="Z805" s="3"/>
     </row>
     <row r="806" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z806" s="2"/>
+      <c r="Z806" s="3"/>
     </row>
     <row r="807" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z807" s="2"/>
+      <c r="Z807" s="3"/>
     </row>
     <row r="808" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z808" s="2"/>
+      <c r="Z808" s="3"/>
     </row>
     <row r="809" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z809" s="2"/>
+      <c r="Z809" s="3"/>
     </row>
     <row r="810" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z810" s="2"/>
+      <c r="Z810" s="3"/>
     </row>
     <row r="811" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z811" s="2"/>
+      <c r="Z811" s="3"/>
     </row>
     <row r="812" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z812" s="2"/>
+      <c r="Z812" s="3"/>
     </row>
     <row r="813" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z813" s="2"/>
+      <c r="Z813" s="3"/>
     </row>
     <row r="814" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z814" s="2"/>
+      <c r="Z814" s="3"/>
     </row>
     <row r="815" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z815" s="2"/>
+      <c r="Z815" s="3"/>
     </row>
     <row r="816" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z816" s="2"/>
+      <c r="Z816" s="3"/>
     </row>
     <row r="817" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z817" s="2"/>
+      <c r="Z817" s="3"/>
     </row>
     <row r="818" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z818" s="2"/>
+      <c r="Z818" s="3"/>
     </row>
     <row r="819" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z819" s="2"/>
+      <c r="Z819" s="3"/>
     </row>
     <row r="820" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z820" s="2"/>
+      <c r="Z820" s="3"/>
     </row>
     <row r="821" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z821" s="2"/>
+      <c r="Z821" s="3"/>
     </row>
     <row r="822" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z822" s="2"/>
+      <c r="Z822" s="3"/>
     </row>
     <row r="823" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z823" s="2"/>
+      <c r="Z823" s="3"/>
     </row>
     <row r="824" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z824" s="2"/>
+      <c r="Z824" s="3"/>
     </row>
     <row r="825" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z825" s="2"/>
+      <c r="Z825" s="3"/>
     </row>
     <row r="826" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z826" s="2"/>
+      <c r="Z826" s="3"/>
     </row>
     <row r="827" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z827" s="2"/>
+      <c r="Z827" s="3"/>
     </row>
     <row r="828" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z828" s="2"/>
+      <c r="Z828" s="3"/>
     </row>
     <row r="829" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z829" s="2"/>
+      <c r="Z829" s="3"/>
     </row>
     <row r="830" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z830" s="2"/>
+      <c r="Z830" s="3"/>
     </row>
     <row r="831" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z831" s="2"/>
+      <c r="Z831" s="3"/>
     </row>
     <row r="832" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z832" s="2"/>
+      <c r="Z832" s="3"/>
     </row>
     <row r="833" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z833" s="2"/>
+      <c r="Z833" s="3"/>
     </row>
     <row r="834" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z834" s="2"/>
+      <c r="Z834" s="3"/>
     </row>
     <row r="835" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z835" s="2"/>
+      <c r="Z835" s="3"/>
     </row>
     <row r="836" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z836" s="2"/>
+      <c r="Z836" s="3"/>
     </row>
     <row r="837" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z837" s="2"/>
+      <c r="Z837" s="3"/>
     </row>
     <row r="838" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z838" s="2"/>
+      <c r="Z838" s="3"/>
     </row>
     <row r="839" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z839" s="2"/>
+      <c r="Z839" s="3"/>
     </row>
     <row r="840" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z840" s="2"/>
+      <c r="Z840" s="3"/>
     </row>
     <row r="841" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z841" s="2"/>
+      <c r="Z841" s="3"/>
     </row>
     <row r="842" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Z842" s="2"/>
+      <c r="Z842" s="3"/>
     </row>
     <row r="1048011" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048012" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>